<commit_message>
Fix order search qty issue
</commit_message>
<xml_diff>
--- a/public/xlsx/example_order.xlsx
+++ b/public/xlsx/example_order.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christiansky\Documents\!sites\wow\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christiansky\Documents\!sites\reports_new\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="38">
   <si>
     <t>phone</t>
   </si>
@@ -124,6 +124,18 @@
   </si>
   <si>
     <t>nocod</t>
+  </si>
+  <si>
+    <t>shipping_method</t>
+  </si>
+  <si>
+    <t>inout2</t>
+  </si>
+  <si>
+    <t>crossborder</t>
+  </si>
+  <si>
+    <t>Athens</t>
   </si>
 </sst>
 </file>
@@ -236,7 +248,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -271,7 +283,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -480,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,17 +508,17 @@
     <col min="6" max="6" width="40.5703125" customWidth="1"/>
     <col min="7" max="7" width="33.42578125" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" customWidth="1"/>
-    <col min="9" max="9" width="17.140625" customWidth="1"/>
-    <col min="10" max="10" width="21.85546875" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" customWidth="1"/>
-    <col min="12" max="12" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27" customWidth="1"/>
-    <col min="15" max="15" width="31.42578125" customWidth="1"/>
-    <col min="16" max="16" width="113.85546875" customWidth="1"/>
+    <col min="9" max="10" width="17.140625" customWidth="1"/>
+    <col min="11" max="11" width="21.85546875" customWidth="1"/>
+    <col min="12" max="12" width="20.140625" customWidth="1"/>
+    <col min="13" max="13" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27" customWidth="1"/>
+    <col min="16" max="16" width="31.42578125" customWidth="1"/>
+    <col min="17" max="17" width="113.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
@@ -535,28 +547,31 @@
         <v>6</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>7</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>8</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10001</v>
       </c>
@@ -584,29 +599,29 @@
       <c r="I2" t="s">
         <v>12</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>14</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>1</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>57.9</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10001</v>
       </c>
@@ -634,29 +649,29 @@
       <c r="I3" t="s">
         <v>12</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>16</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>3</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>57.9</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10001</v>
       </c>
@@ -684,29 +699,29 @@
       <c r="I4" t="s">
         <v>12</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>17</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>1</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>57.9</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>15</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="Q4" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>10002</v>
       </c>
@@ -731,23 +746,23 @@
       <c r="I5" t="s">
         <v>12</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>14</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>2</v>
       </c>
-      <c r="P5" s="2" t="s">
+      <c r="Q5" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>10003</v>
       </c>
@@ -772,27 +787,103 @@
       <c r="I6" t="s">
         <v>19</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>14</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>1</v>
       </c>
-      <c r="P6" s="2" t="s">
+      <c r="Q6" s="2" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>10009</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7">
+        <v>548214</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7">
+        <v>10673</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M7" t="s">
+        <v>16</v>
+      </c>
+      <c r="N7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>10009</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8">
+        <v>548214</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8">
+        <v>10673</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M8" t="s">
+        <v>17</v>
+      </c>
+      <c r="N8">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <hyperlinks>
-    <hyperlink ref="P2" r:id="rId1"/>
-    <hyperlink ref="P3:P6" r:id="rId2" display="https://example.com/document.pdf"/>
+    <hyperlink ref="Q2" r:id="rId1"/>
+    <hyperlink ref="Q3:Q6" r:id="rId2" display="https://example.com/document.pdf"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId3"/>

</xml_diff>

<commit_message>
Order adding product bugfiing
</commit_message>
<xml_diff>
--- a/public/xlsx/example_order.xlsx
+++ b/public/xlsx/example_order.xlsx
@@ -5,24 +5,24 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christiansky\Documents\!sites\reports_new\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christiansky\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" tabRatio="159"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13680" tabRatio="159"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Worksheet!$H$1:$I$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Worksheet!$J$1:$K$1</definedName>
   </definedNames>
-  <calcPr calcId="162913" forceFullCalc="1"/>
+  <calcPr calcId="162913" iterateDelta="1E-4" forceFullCalc="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="49">
   <si>
     <t>phone</t>
   </si>
@@ -87,9 +87,6 @@
     <t>Пловдив</t>
   </si>
   <si>
-    <t>Улица</t>
-  </si>
-  <si>
     <t>Пример Пример</t>
   </si>
   <si>
@@ -136,6 +133,42 @@
   </si>
   <si>
     <t>Athens</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>example@metrica.bg</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>BG</t>
+  </si>
+  <si>
+    <t>GR</t>
+  </si>
+  <si>
+    <t>Street name 123</t>
+  </si>
+  <si>
+    <t>street name 8998</t>
+  </si>
+  <si>
+    <t>street name 88663</t>
+  </si>
+  <si>
+    <t>Street Test 996</t>
+  </si>
+  <si>
+    <t>Delivery instructions</t>
+  </si>
+  <si>
+    <t>Example Name</t>
+  </si>
+  <si>
+    <t>FirstName LastName</t>
   </si>
 </sst>
 </file>
@@ -492,400 +525,458 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q8"/>
+  <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.140625" customWidth="1"/>
     <col min="2" max="2" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
-    <col min="6" max="6" width="40.5703125" customWidth="1"/>
-    <col min="7" max="7" width="33.42578125" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" customWidth="1"/>
-    <col min="9" max="10" width="17.140625" customWidth="1"/>
-    <col min="11" max="11" width="21.85546875" customWidth="1"/>
-    <col min="12" max="12" width="20.140625" customWidth="1"/>
-    <col min="13" max="13" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="27" customWidth="1"/>
-    <col min="16" max="16" width="31.42578125" customWidth="1"/>
-    <col min="17" max="17" width="113.85546875" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
+    <col min="8" max="8" width="40.5703125" customWidth="1"/>
+    <col min="9" max="9" width="33.42578125" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" customWidth="1"/>
+    <col min="11" max="12" width="17.140625" customWidth="1"/>
+    <col min="13" max="13" width="21.85546875" customWidth="1"/>
+    <col min="14" max="14" width="20.140625" customWidth="1"/>
+    <col min="15" max="15" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="27" customWidth="1"/>
+    <col min="18" max="18" width="31.42578125" customWidth="1"/>
+    <col min="19" max="19" width="113.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>7</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10001</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2">
+        <v>123456</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2">
+        <v>7000</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2">
+        <v>714</v>
+      </c>
+      <c r="K2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C2">
-        <v>123456</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2">
-        <v>7000</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2">
-        <v>714</v>
-      </c>
-      <c r="I2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" t="s">
-        <v>13</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>14</v>
       </c>
-      <c r="N2">
+      <c r="P2">
         <v>1</v>
       </c>
-      <c r="O2">
+      <c r="Q2">
         <v>57.9</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="2" t="s">
-        <v>26</v>
+      <c r="S2" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10001</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3">
+        <v>48</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3">
         <v>123456</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="E3">
+      <c r="F3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3">
         <v>7000</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="H3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" t="s">
         <v>11</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <v>714</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>12</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M3" t="s">
+      <c r="N3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O3" t="s">
         <v>16</v>
       </c>
-      <c r="N3">
+      <c r="P3">
         <v>3</v>
       </c>
-      <c r="O3">
+      <c r="Q3">
         <v>57.9</v>
       </c>
-      <c r="P3" t="s">
+      <c r="R3" t="s">
         <v>15</v>
       </c>
-      <c r="Q3" s="2" t="s">
-        <v>26</v>
+      <c r="S3" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10001</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4">
+        <v>48</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4">
         <v>132456</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>10</v>
       </c>
-      <c r="E4">
+      <c r="F4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4">
         <v>7000</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="H4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4" t="s">
         <v>11</v>
       </c>
-      <c r="H4">
+      <c r="J4">
         <v>714</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K4" t="s">
         <v>12</v>
       </c>
-      <c r="K4" t="s">
+      <c r="M4" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="N4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O4" t="s">
+        <v>17</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>57.9</v>
+      </c>
+      <c r="R4" t="s">
+        <v>15</v>
+      </c>
+      <c r="S4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="M4" t="s">
-        <v>17</v>
-      </c>
-      <c r="N4">
-        <v>1</v>
-      </c>
-      <c r="O4">
-        <v>57.9</v>
-      </c>
-      <c r="P4" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>26</v>
-      </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>10002</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5">
+        <v>321654</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5">
+        <v>1000</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5">
+        <v>9006</v>
+      </c>
+      <c r="K5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C5">
-        <v>321654</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5">
-        <v>1000</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5">
-        <v>9006</v>
-      </c>
-      <c r="I5" t="s">
-        <v>12</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M5" t="s">
+      <c r="O5" t="s">
         <v>14</v>
       </c>
-      <c r="N5">
+      <c r="P5">
         <v>2</v>
       </c>
-      <c r="Q5" s="2" t="s">
-        <v>26</v>
+      <c r="S5" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>10003</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6">
+        <v>456321</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6">
+        <v>4000</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J6">
+        <v>4706</v>
+      </c>
+      <c r="K6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C6">
-        <v>456321</v>
-      </c>
-      <c r="D6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6">
-        <v>4000</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6">
-        <v>4706</v>
-      </c>
-      <c r="I6" t="s">
-        <v>19</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M6" t="s">
+      <c r="O6" t="s">
         <v>14</v>
       </c>
-      <c r="N6">
+      <c r="P6">
         <v>1</v>
       </c>
-      <c r="Q6" s="2" t="s">
-        <v>26</v>
+      <c r="S6" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>10009</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7">
+        <v>47</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7">
         <v>548214</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7">
+      <c r="E7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7">
         <v>10673</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>21</v>
+      <c r="H7" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="I7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M7" t="s">
+      <c r="M7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O7" t="s">
         <v>16</v>
       </c>
-      <c r="N7">
+      <c r="P7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>10009</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8">
+        <v>47</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8">
         <v>548214</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8">
+      <c r="E8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8">
         <v>10673</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>21</v>
+      <c r="H8" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="I8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M8" t="s">
+      <c r="M8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O8" t="s">
         <v>17</v>
       </c>
-      <c r="N8">
+      <c r="P8">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <hyperlinks>
-    <hyperlink ref="Q2" r:id="rId1"/>
-    <hyperlink ref="Q3:Q6" r:id="rId2" display="https://example.com/document.pdf"/>
+    <hyperlink ref="S2" r:id="rId1"/>
+    <hyperlink ref="S3:S6" r:id="rId2" display="https://example.com/document.pdf"/>
+    <hyperlink ref="C2" r:id="rId3"/>
+    <hyperlink ref="C3:C8" r:id="rId4" display="example@metrica.bg"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>